<commit_message>
Empecé a desarrollar la validación del CSV.
</commit_message>
<xml_diff>
--- a/Recursos/Insumo.xlsx
+++ b/Recursos/Insumo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blandonm\Documents\Proyectos RPA NumRot\HabilitacionDeEmpresasRPA\HabilitacionDeEmpresasRPA\Recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FE6263A-F341-48D4-9919-435B98CD23B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DFBACF8-2B31-47D6-A586-89ACBE5E319D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6924F7CD-6230-4835-BB24-1BCA0C910BD6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>THE POWER OF LOVE S.A.S</t>
   </si>
@@ -49,6 +49,12 @@
   </si>
   <si>
     <t>SETID</t>
+  </si>
+  <si>
+    <t>NIT DE EMPRESA PADRE</t>
+  </si>
+  <si>
+    <t>AMBIENTE (1 PARA FACTURA/2 PARA NÓMINA)</t>
   </si>
 </sst>
 </file>
@@ -415,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08ACCA7-4E7D-4E6E-879D-F792D98795A8}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,9 +433,10 @@
     <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="43.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -442,8 +449,14 @@
       <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -456,8 +469,14 @@
       <c r="D2" t="s">
         <v>1</v>
       </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>98561334</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -469,6 +488,12 @@
       </c>
       <c r="D3" t="s">
         <v>2</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>98561334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Hasta este punto logré hacer inserción de factura a base de datos SQLite3.
</commit_message>
<xml_diff>
--- a/Recursos/Insumo.xlsx
+++ b/Recursos/Insumo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blandonm\Documents\Proyectos RPA NumRot\HabilitacionDeEmpresasRPA\HabilitacionDeEmpresasRPA\Recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DFBACF8-2B31-47D6-A586-89ACBE5E319D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{662F337A-7260-4B75-8187-B5CCD7BD2E4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6924F7CD-6230-4835-BB24-1BCA0C910BD6}"/>
   </bookViews>
@@ -25,18 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>THE POWER OF LOVE S.A.S</t>
   </si>
   <si>
     <t>6e3c6c47-451f-4bbe-acb4-a58ab2c7d166</t>
-  </si>
-  <si>
-    <t>6e3c6c47-451f-4bbe-acb4-a58ab2c7d167</t>
-  </si>
-  <si>
-    <t>FONDO FEPEP</t>
   </si>
   <si>
     <t>RAZÓN SOCIAL</t>
@@ -421,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08ACCA7-4E7D-4E6E-879D-F792D98795A8}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,22 +432,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -473,26 +467,6 @@
         <v>2</v>
       </c>
       <c r="F2">
-        <v>98561334</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>901582324</v>
-      </c>
-      <c r="C3">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
         <v>98561334</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Continúa desarrollo. He agragado condición para cuando es nómina en algunas de las secuencias.
</commit_message>
<xml_diff>
--- a/Recursos/Insumo.xlsx
+++ b/Recursos/Insumo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blandonm\Documents\Proyectos RPA NumRot\HabilitacionDeEmpresasRPA\HabilitacionDeEmpresasRPA\Recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{662F337A-7260-4B75-8187-B5CCD7BD2E4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15AADED0-6332-494F-96C0-F4373D74BCED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6924F7CD-6230-4835-BB24-1BCA0C910BD6}"/>
+    <workbookView xWindow="10995" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{6924F7CD-6230-4835-BB24-1BCA0C910BD6}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>THE POWER OF LOVE S.A.S</t>
   </si>
@@ -49,6 +49,12 @@
   </si>
   <si>
     <t>AMBIENTE (1 PARA FACTURA/2 PARA NÓMINA)</t>
+  </si>
+  <si>
+    <t>CLINICA ODONTOLOGICA Y ESTETICA JEINNER GUERRA S.A.S.</t>
+  </si>
+  <si>
+    <t>23726609-f9ce-47dc-9cc6-098578a7fe36</t>
   </si>
 </sst>
 </file>
@@ -415,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08ACCA7-4E7D-4E6E-879D-F792D98795A8}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,8 +476,29 @@
         <v>98561334</v>
       </c>
     </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>901740209</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>76090231</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Completada la versión 1.0 de la automatización para habilitar empresa.
</commit_message>
<xml_diff>
--- a/Recursos/Insumo.xlsx
+++ b/Recursos/Insumo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blandonm\Documents\Proyectos RPA NumRot\HabilitacionDeEmpresasRPA\HabilitacionDeEmpresasRPA\Recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15AADED0-6332-494F-96C0-F4373D74BCED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D76A2C-2059-454E-A6F3-BB529D769D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10995" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{6924F7CD-6230-4835-BB24-1BCA0C910BD6}"/>
+    <workbookView xWindow="10440" yWindow="-16455" windowWidth="29040" windowHeight="15840" xr2:uid="{6924F7CD-6230-4835-BB24-1BCA0C910BD6}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,12 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
-    <t>THE POWER OF LOVE S.A.S</t>
-  </si>
-  <si>
-    <t>6e3c6c47-451f-4bbe-acb4-a58ab2c7d166</t>
-  </si>
-  <si>
     <t>RAZÓN SOCIAL</t>
   </si>
   <si>
@@ -55,6 +49,12 @@
   </si>
   <si>
     <t>23726609-f9ce-47dc-9cc6-098578a7fe36</t>
+  </si>
+  <si>
+    <t>INVERSIONES IOWA SAS</t>
+  </si>
+  <si>
+    <t>e58a834e-0159-4e8b-97a4-c9fb59bee78a</t>
   </si>
 </sst>
 </file>
@@ -424,7 +424,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,36 +438,36 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B2">
-        <v>901582324</v>
+        <v>901625453</v>
       </c>
       <c r="C2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -478,7 +478,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>901740209</v>
@@ -487,7 +487,7 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E3">
         <v>1</v>

</xml_diff>